<commit_message>
Mise à jour du fichier via Shiny
</commit_message>
<xml_diff>
--- a/PIB_va.xlsx
+++ b/PIB_va.xlsx
@@ -989,15 +989,15 @@
         <v>140421.038374167</v>
       </c>
       <c r="T2" t="n">
-        <v>258013.949237456</v>
+        <v>158976.24949317</v>
       </c>
       <c r="U2" t="n">
-        <v>4598133.63771179</v>
+        <v>4499095.9379675</v>
       </c>
       <c r="V2"/>
       <c r="W2"/>
       <c r="X2" t="n">
-        <v>18938356.3274427</v>
+        <v>18538316.6234983</v>
       </c>
       <c r="Y2"/>
     </row>
@@ -1060,17 +1060,17 @@
         <v>141159.814181197</v>
       </c>
       <c r="T3" t="n">
-        <v>266479.233262062</v>
+        <v>167863.759123018</v>
       </c>
       <c r="U3" t="n">
-        <v>4713845.70114401</v>
+        <v>4615230.22700496</v>
       </c>
       <c r="V3" t="n">
-        <v>2.51650066199036</v>
+        <v>2.58128056477775</v>
       </c>
       <c r="W3"/>
       <c r="X3" t="n">
-        <v>18938356.3274427</v>
+        <v>18538316.6234983</v>
       </c>
       <c r="Y3"/>
     </row>
@@ -1133,17 +1133,17 @@
         <v>142637.365795258</v>
       </c>
       <c r="T4" t="n">
-        <v>263611.788326039</v>
+        <v>160518.615580187</v>
       </c>
       <c r="U4" t="n">
-        <v>4654457.81482471</v>
+        <v>4551364.64207886</v>
       </c>
       <c r="V4" t="n">
-        <v>-1.25986063364115</v>
+        <v>-1.38380062932532</v>
       </c>
       <c r="W4"/>
       <c r="X4" t="n">
-        <v>18938356.3274427</v>
+        <v>18538316.6234983</v>
       </c>
       <c r="Y4"/>
     </row>
@@ -1206,17 +1206,17 @@
         <v>144853.693216349</v>
       </c>
       <c r="T5" t="n">
-        <v>298430.733118788</v>
+        <v>199137.375803625</v>
       </c>
       <c r="U5" t="n">
-        <v>4971919.17376216</v>
+        <v>4872625.81644699</v>
       </c>
       <c r="V5" t="n">
-        <v>6.82058730721148</v>
+        <v>7.05856813576244</v>
       </c>
       <c r="W5"/>
       <c r="X5" t="n">
-        <v>18938356.3274427</v>
+        <v>18538316.6234983</v>
       </c>
       <c r="Y5"/>
     </row>
@@ -1279,22 +1279,22 @@
         <v>139156.484965668</v>
       </c>
       <c r="T6" t="n">
-        <v>272899.864033571</v>
+        <v>177927.251417037</v>
       </c>
       <c r="U6" t="n">
-        <v>4904379.75136973</v>
+        <v>4809407.13875319</v>
       </c>
       <c r="V6" t="n">
-        <v>-1.35841754525792</v>
+        <v>-1.29742525027086</v>
       </c>
       <c r="W6" t="n">
-        <v>6.66022646984959</v>
+        <v>6.89719012584282</v>
       </c>
       <c r="X6" t="n">
-        <v>20267121.3403819</v>
+        <v>19888829.7931632</v>
       </c>
       <c r="Y6" t="n">
-        <v>7.01626366071589</v>
+        <v>7.28498275810583</v>
       </c>
     </row>
     <row r="7">
@@ -1356,22 +1356,22 @@
         <v>139998.733180159</v>
       </c>
       <c r="T7" t="n">
-        <v>282322.500619949</v>
+        <v>186717.608258595</v>
       </c>
       <c r="U7" t="n">
-        <v>5069186.42487102</v>
+        <v>4973581.53250967</v>
       </c>
       <c r="V7" t="n">
-        <v>3.36039788630287</v>
+        <v>3.41360980719623</v>
       </c>
       <c r="W7" t="n">
-        <v>7.53823409282947</v>
+        <v>7.76453801606458</v>
       </c>
       <c r="X7" t="n">
-        <v>20267121.3403819</v>
+        <v>19888829.7931632</v>
       </c>
       <c r="Y7" t="n">
-        <v>7.01626366071589</v>
+        <v>7.28498275810583</v>
       </c>
     </row>
     <row r="8">
@@ -1433,22 +1433,22 @@
         <v>138728.126381018</v>
       </c>
       <c r="T8" t="n">
-        <v>268493.428329449</v>
+        <v>170254.109991386</v>
       </c>
       <c r="U8" t="n">
-        <v>4976666.15197925</v>
+        <v>4878426.83364119</v>
       </c>
       <c r="V8" t="n">
-        <v>-1.82515033256304</v>
+        <v>-1.91320275432315</v>
       </c>
       <c r="W8" t="n">
-        <v>6.92257508765656</v>
+        <v>7.1860247921806</v>
       </c>
       <c r="X8" t="n">
-        <v>20267121.3403819</v>
+        <v>19888829.7931632</v>
       </c>
       <c r="Y8" t="n">
-        <v>7.01626366071589</v>
+        <v>7.28498275810583</v>
       </c>
     </row>
     <row r="9">
@@ -1510,22 +1510,22 @@
         <v>135344.664568246</v>
       </c>
       <c r="T9" t="n">
-        <v>281264.019322242</v>
+        <v>191789.295419521</v>
       </c>
       <c r="U9" t="n">
-        <v>5316889.01216191</v>
+        <v>5227414.28825919</v>
       </c>
       <c r="V9" t="n">
-        <v>6.83636092502114</v>
+        <v>7.15368840240502</v>
       </c>
       <c r="W9" t="n">
-        <v>6.9383637654496</v>
+        <v>7.28125830254907</v>
       </c>
       <c r="X9" t="n">
-        <v>20267121.3403819</v>
+        <v>19888829.7931632</v>
       </c>
       <c r="Y9" t="n">
-        <v>7.01626366071589</v>
+        <v>7.28498275810583</v>
       </c>
     </row>
     <row r="10">
@@ -1587,22 +1587,22 @@
         <v>128124.13020758</v>
       </c>
       <c r="T10" t="n">
-        <v>248325.937099972</v>
+        <v>158716.094239957</v>
       </c>
       <c r="U10" t="n">
-        <v>5132324.37062395</v>
+        <v>5042714.52776394</v>
       </c>
       <c r="V10" t="n">
-        <v>-3.47129009305597</v>
+        <v>-3.5332910366429</v>
       </c>
       <c r="W10" t="n">
-        <v>4.64777669776822</v>
+        <v>4.85106339055395</v>
       </c>
       <c r="X10" t="n">
-        <v>20749004.5077808</v>
+        <v>20382823.3270026</v>
       </c>
       <c r="Y10" t="n">
-        <v>2.37765965528994</v>
+        <v>2.48377375127989</v>
       </c>
     </row>
     <row r="11">
@@ -1664,22 +1664,22 @@
         <v>127685.829284415</v>
       </c>
       <c r="T11" t="n">
-        <v>242320.002939513</v>
+        <v>154949.248673669</v>
       </c>
       <c r="U11" t="n">
-        <v>5195863.23804144</v>
+        <v>5108492.4837756</v>
       </c>
       <c r="V11" t="n">
-        <v>1.23801347750284</v>
+        <v>1.30441562078324</v>
       </c>
       <c r="W11" t="n">
-        <v>2.49895747666533</v>
+        <v>2.71255131506515</v>
       </c>
       <c r="X11" t="n">
-        <v>20749004.5077808</v>
+        <v>20382823.3270026</v>
       </c>
       <c r="Y11" t="n">
-        <v>2.37765965528994</v>
+        <v>2.48377375127989</v>
       </c>
     </row>
     <row r="12">
@@ -1741,22 +1741,22 @@
         <v>132305.544264488</v>
       </c>
       <c r="T12" t="n">
-        <v>215874.882206094</v>
+        <v>119522.315539505</v>
       </c>
       <c r="U12" t="n">
-        <v>5234036.3152766</v>
+        <v>5137683.74861002</v>
       </c>
       <c r="V12" t="n">
-        <v>0.734682101631938</v>
+        <v>0.571426206990211</v>
       </c>
       <c r="W12" t="n">
-        <v>5.17153764061506</v>
+        <v>5.31435488959305</v>
       </c>
       <c r="X12" t="n">
-        <v>20749004.5077808</v>
+        <v>20382823.3270026</v>
       </c>
       <c r="Y12" t="n">
-        <v>2.37765965528994</v>
+        <v>2.48377375127989</v>
       </c>
     </row>
     <row r="13">
@@ -1818,22 +1818,22 @@
         <v>141983.275147799</v>
       </c>
       <c r="T13" t="n">
-        <v>257179.881541653</v>
+        <v>164331.864555832</v>
       </c>
       <c r="U13" t="n">
-        <v>5186780.58383883</v>
+        <v>5093932.56685301</v>
       </c>
       <c r="V13" t="n">
-        <v>-0.902854481537434</v>
+        <v>-0.851574053557515</v>
       </c>
       <c r="W13" t="n">
-        <v>-2.44707813207059</v>
+        <v>-2.55349421426152</v>
       </c>
       <c r="X13" t="n">
-        <v>20749004.5077808</v>
+        <v>20382823.3270026</v>
       </c>
       <c r="Y13" t="n">
-        <v>2.37765965528994</v>
+        <v>2.48377375127989</v>
       </c>
     </row>
     <row r="14">
@@ -1895,22 +1895,22 @@
         <v>154201.993515976</v>
       </c>
       <c r="T14" t="n">
-        <v>234892.915362819</v>
+        <v>156479.414649205</v>
       </c>
       <c r="U14" t="n">
-        <v>5155434.32036764</v>
+        <v>5077020.81965402</v>
       </c>
       <c r="V14" t="n">
-        <v>-0.604349132655881</v>
+        <v>-0.331997861711679</v>
       </c>
       <c r="W14" t="n">
-        <v>0.450282329697659</v>
+        <v>0.680313979726686</v>
       </c>
       <c r="X14" t="n">
-        <v>20203091.9858354</v>
+        <v>19879480.2704067</v>
       </c>
       <c r="Y14" t="n">
-        <v>-2.63102994527161</v>
+        <v>-2.46944718364437</v>
       </c>
     </row>
     <row r="15">
@@ -1972,22 +1972,22 @@
         <v>163378.379728023</v>
       </c>
       <c r="T15" t="n">
-        <v>242502.372055104</v>
+        <v>159635.690033202</v>
       </c>
       <c r="U15" t="n">
-        <v>5265217.03579075</v>
+        <v>5182350.35376885</v>
       </c>
       <c r="V15" t="n">
-        <v>2.12945619323273</v>
+        <v>2.07463270008818</v>
       </c>
       <c r="W15" t="n">
-        <v>1.33478874581495</v>
+        <v>1.44578601667372</v>
       </c>
       <c r="X15" t="n">
-        <v>20203091.9858354</v>
+        <v>19879480.2704067</v>
       </c>
       <c r="Y15" t="n">
-        <v>-2.63102994527161</v>
+        <v>-2.46944718364437</v>
       </c>
     </row>
     <row r="16">
@@ -2049,22 +2049,22 @@
         <v>166995.405365568</v>
       </c>
       <c r="T16" t="n">
-        <v>230227.824727722</v>
+        <v>144389.471024191</v>
       </c>
       <c r="U16" t="n">
-        <v>4929673.72891202</v>
+        <v>4843835.37520849</v>
       </c>
       <c r="V16" t="n">
-        <v>-6.37282954525608</v>
+        <v>-6.53207435723011</v>
       </c>
       <c r="W16" t="n">
-        <v>-5.81506447473885</v>
+        <v>-5.71947180441035</v>
       </c>
       <c r="X16" t="n">
-        <v>20203091.9858354</v>
+        <v>19879480.2704067</v>
       </c>
       <c r="Y16" t="n">
-        <v>-2.63102994527161</v>
+        <v>-2.46944718364437</v>
       </c>
     </row>
     <row r="17">
@@ -2126,22 +2126,22 @@
         <v>165053.07042861</v>
       </c>
       <c r="T17" t="n">
-        <v>238375.943695122</v>
+        <v>161882.764705498</v>
       </c>
       <c r="U17" t="n">
-        <v>4852766.90076494</v>
+        <v>4776273.72177532</v>
       </c>
       <c r="V17" t="n">
-        <v>-1.56007947739079</v>
+        <v>-1.39479664769298</v>
       </c>
       <c r="W17" t="n">
-        <v>-6.43971106305562</v>
+        <v>-6.23602375784767</v>
       </c>
       <c r="X17" t="n">
-        <v>20203091.9858354</v>
+        <v>19879480.2704067</v>
       </c>
       <c r="Y17" t="n">
-        <v>-2.63102994527161</v>
+        <v>-2.46944718364437</v>
       </c>
     </row>
     <row r="18">
@@ -2203,22 +2203,22 @@
         <v>170559.19484922</v>
       </c>
       <c r="T18" t="n">
-        <v>231599.192496633</v>
+        <v>166953.82472187</v>
       </c>
       <c r="U18" t="n">
-        <v>4831819.73894794</v>
+        <v>4767174.37117317</v>
       </c>
       <c r="V18" t="n">
-        <v>-0.431653987206843</v>
+        <v>-0.190511497711278</v>
       </c>
       <c r="W18" t="n">
-        <v>-6.27715457728158</v>
+        <v>-6.10291861087869</v>
       </c>
       <c r="X18" t="n">
-        <v>19910780.1541272</v>
+        <v>19666295.0716987</v>
       </c>
       <c r="Y18" t="n">
-        <v>-1.44686680589847</v>
+        <v>-1.07238819027539</v>
       </c>
     </row>
     <row r="19">
@@ -2280,22 +2280,22 @@
         <v>165233.306005293</v>
       </c>
       <c r="T19" t="n">
-        <v>223162.611337962</v>
+        <v>163135.073677866</v>
       </c>
       <c r="U19" t="n">
-        <v>5071020.75436997</v>
+        <v>5010993.21670987</v>
       </c>
       <c r="V19" t="n">
-        <v>4.95053682350565</v>
+        <v>5.11453591903535</v>
       </c>
       <c r="W19" t="n">
-        <v>-3.68828635364354</v>
+        <v>-3.30655253623213</v>
       </c>
       <c r="X19" t="n">
-        <v>19910780.1541272</v>
+        <v>19666295.0716987</v>
       </c>
       <c r="Y19" t="n">
-        <v>-1.44686680589847</v>
+        <v>-1.07238819027539</v>
       </c>
     </row>
     <row r="20">
@@ -2357,22 +2357,22 @@
         <v>162083.223828898</v>
       </c>
       <c r="T20" t="n">
-        <v>211523.52635164</v>
+        <v>148157.132876117</v>
       </c>
       <c r="U20" t="n">
-        <v>4973211.99316748</v>
+        <v>4909845.59969196</v>
       </c>
       <c r="V20" t="n">
-        <v>-1.9287785623476</v>
+        <v>-2.01851434722804</v>
       </c>
       <c r="W20" t="n">
-        <v>0.883187542415069</v>
+        <v>1.36276771133301</v>
       </c>
       <c r="X20" t="n">
-        <v>19910780.1541272</v>
+        <v>19666295.0716987</v>
       </c>
       <c r="Y20" t="n">
-        <v>-1.44686680589847</v>
+        <v>-1.07238819027539</v>
       </c>
     </row>
     <row r="21">
@@ -2434,22 +2434,22 @@
         <v>161108.948320037</v>
       </c>
       <c r="T21" t="n">
-        <v>264444.706406879</v>
+        <v>207998.922888808</v>
       </c>
       <c r="U21" t="n">
-        <v>5034727.66764178</v>
+        <v>4978281.88412371</v>
       </c>
       <c r="V21" t="n">
-        <v>1.23694052372623</v>
+        <v>1.39385817827036</v>
       </c>
       <c r="W21" t="n">
-        <v>3.74962924446588</v>
+        <v>4.22940924485607</v>
       </c>
       <c r="X21" t="n">
-        <v>19910780.1541272</v>
+        <v>19666295.0716987</v>
       </c>
       <c r="Y21" t="n">
-        <v>-1.44686680589847</v>
+        <v>-1.07238819027539</v>
       </c>
     </row>
     <row r="22">
@@ -2511,22 +2511,22 @@
         <v>163328.610000504</v>
       </c>
       <c r="T22" t="n">
-        <v>254981.462133413</v>
+        <v>199644.370166862</v>
       </c>
       <c r="U22" t="n">
-        <v>4949616.82935923</v>
+        <v>4894279.73739268</v>
       </c>
       <c r="V22" t="n">
-        <v>-1.69047551130837</v>
+        <v>-1.6873722438041</v>
       </c>
       <c r="W22" t="n">
-        <v>2.43794464147261</v>
+        <v>2.66626215705698</v>
       </c>
       <c r="X22" t="n">
-        <v>19240671.4385308</v>
+        <v>19002919.2057614</v>
       </c>
       <c r="Y22" t="n">
-        <v>-3.36555730317526</v>
+        <v>-3.37316135814515</v>
       </c>
     </row>
     <row r="23">
@@ -2588,22 +2588,22 @@
         <v>164196.038063109</v>
       </c>
       <c r="T23" t="n">
-        <v>261217.332532871</v>
+        <v>199149.515219265</v>
       </c>
       <c r="U23" t="n">
-        <v>5038288.04320805</v>
+        <v>4976220.22589444</v>
       </c>
       <c r="V23" t="n">
-        <v>1.79147632848772</v>
+        <v>1.67420934025753</v>
       </c>
       <c r="W23" t="n">
-        <v>-0.645485647711308</v>
+        <v>-0.693934102713898</v>
       </c>
       <c r="X23" t="n">
-        <v>19240671.4385308</v>
+        <v>19002919.2057614</v>
       </c>
       <c r="Y23" t="n">
-        <v>-3.36555730317526</v>
+        <v>-3.37316135814515</v>
       </c>
     </row>
     <row r="24">
@@ -2665,22 +2665,22 @@
         <v>164729.363029647</v>
       </c>
       <c r="T24" t="n">
-        <v>252116.107245682</v>
+        <v>185189.113202237</v>
       </c>
       <c r="U24" t="n">
-        <v>4790569.73576326</v>
+        <v>4723642.74171981</v>
       </c>
       <c r="V24" t="n">
-        <v>-4.91671586301483</v>
+        <v>-5.0756894331225</v>
       </c>
       <c r="W24" t="n">
-        <v>-3.6725210518906</v>
+        <v>-3.79243815699272</v>
       </c>
       <c r="X24" t="n">
-        <v>19240671.4385308</v>
+        <v>19002919.2057614</v>
       </c>
       <c r="Y24" t="n">
-        <v>-3.36555730317526</v>
+        <v>-3.37316135814515</v>
       </c>
     </row>
     <row r="25">
@@ -2742,22 +2742,22 @@
         <v>164928.58490012</v>
       </c>
       <c r="T25" t="n">
-        <v>289035.364030953</v>
+        <v>235615.034585149</v>
       </c>
       <c r="U25" t="n">
-        <v>4462196.83020024</v>
+        <v>4408776.50075443</v>
       </c>
       <c r="V25" t="n">
-        <v>-6.85456894848238</v>
+        <v>-6.66575052733018</v>
       </c>
       <c r="W25" t="n">
-        <v>-11.3716346788965</v>
+        <v>-11.4397978383968</v>
       </c>
       <c r="X25" t="n">
-        <v>19240671.4385308</v>
+        <v>19002919.2057614</v>
       </c>
       <c r="Y25" t="n">
-        <v>-3.36555730317526</v>
+        <v>-3.37316135814515</v>
       </c>
     </row>
     <row r="26">
@@ -2819,22 +2819,22 @@
         <v>164597.592214852</v>
       </c>
       <c r="T26" t="n">
-        <v>298757.185315629</v>
+        <v>235945.113575264</v>
       </c>
       <c r="U26" t="n">
-        <v>4370867.20925583</v>
+        <v>4308055.13751547</v>
       </c>
       <c r="V26" t="n">
-        <v>-2.04674119990139</v>
+        <v>-2.2845649631304</v>
       </c>
       <c r="W26" t="n">
-        <v>-11.6928166372491</v>
+        <v>-11.9777501763622</v>
       </c>
       <c r="X26" t="n">
-        <v>17988522.0286624</v>
+        <v>17741261.8388822</v>
       </c>
       <c r="Y26" t="n">
-        <v>-6.50782595539165</v>
+        <v>-6.63928185568806</v>
       </c>
     </row>
     <row r="27">
@@ -2896,22 +2896,22 @@
         <v>165383.935348532</v>
       </c>
       <c r="T27" t="n">
-        <v>266694.527010078</v>
+        <v>201565.885543819</v>
       </c>
       <c r="U27" t="n">
-        <v>4501010.484121</v>
+        <v>4435881.84265474</v>
       </c>
       <c r="V27" t="n">
-        <v>2.97751609999895</v>
+        <v>2.96715573638161</v>
       </c>
       <c r="W27" t="n">
-        <v>-10.6638912757545</v>
+        <v>-10.8584097710944</v>
       </c>
       <c r="X27" t="n">
-        <v>17988522.0286624</v>
+        <v>17741261.8388822</v>
       </c>
       <c r="Y27" t="n">
-        <v>-6.50782595539165</v>
+        <v>-6.63928185568806</v>
       </c>
     </row>
     <row r="28">
@@ -2973,22 +2973,22 @@
         <v>167091.502841485</v>
       </c>
       <c r="T28" t="n">
-        <v>263619.026262331</v>
+        <v>200692.360376997</v>
       </c>
       <c r="U28" t="n">
-        <v>4449950.84694997</v>
+        <v>4387024.18106464</v>
       </c>
       <c r="V28" t="n">
-        <v>-1.13440387111204</v>
+        <v>-1.10141936424671</v>
       </c>
       <c r="W28" t="n">
-        <v>-7.11019581388091</v>
+        <v>-7.12624936009908</v>
       </c>
       <c r="X28" t="n">
-        <v>17988522.0286624</v>
+        <v>17741261.8388822</v>
       </c>
       <c r="Y28" t="n">
-        <v>-6.50782595539165</v>
+        <v>-6.63928185568806</v>
       </c>
     </row>
     <row r="29">
@@ -3050,22 +3050,22 @@
         <v>169720.294693711</v>
       </c>
       <c r="T29" t="n">
-        <v>288836.300182915</v>
+        <v>232443.489494629</v>
       </c>
       <c r="U29" t="n">
-        <v>4666693.48833563</v>
+        <v>4610300.67764735</v>
       </c>
       <c r="V29" t="n">
-        <v>4.87067495440348</v>
+        <v>5.08947494628404</v>
       </c>
       <c r="W29" t="n">
-        <v>4.5828695128677</v>
+        <v>4.57097738700136</v>
       </c>
       <c r="X29" t="n">
-        <v>17988522.0286624</v>
+        <v>17741261.8388822</v>
       </c>
       <c r="Y29" t="n">
-        <v>-6.50782595539165</v>
+        <v>-6.63928185568806</v>
       </c>
     </row>
     <row r="30">
@@ -3127,22 +3127,22 @@
         <v>174316.195281317</v>
       </c>
       <c r="T30" t="n">
-        <v>336853.659437033</v>
+        <v>268578.944041909</v>
       </c>
       <c r="U30" t="n">
-        <v>4415649.01575808</v>
+        <v>4347374.30036296</v>
       </c>
       <c r="V30" t="n">
-        <v>-5.37949349373452</v>
+        <v>-5.70302016437155</v>
       </c>
       <c r="W30" t="n">
-        <v>1.02455197923696</v>
+        <v>0.9126894060638</v>
       </c>
       <c r="X30" t="n">
-        <v>18098575.9924922</v>
+        <v>17832479.0875058</v>
       </c>
       <c r="Y30" t="n">
-        <v>0.611801034317154</v>
+        <v>0.514153105072473</v>
       </c>
     </row>
     <row r="31">
@@ -3204,22 +3204,22 @@
         <v>176134.318905654</v>
       </c>
       <c r="T31" t="n">
-        <v>322381.945510853</v>
+        <v>251955.427601384</v>
       </c>
       <c r="U31" t="n">
-        <v>4654819.98849914</v>
+        <v>4584393.47058967</v>
       </c>
       <c r="V31" t="n">
-        <v>5.41643984581947</v>
+        <v>5.45200743830413</v>
       </c>
       <c r="W31" t="n">
-        <v>3.4172216421348</v>
+        <v>3.34796176279685</v>
       </c>
       <c r="X31" t="n">
-        <v>18098575.9924922</v>
+        <v>17832479.0875058</v>
       </c>
       <c r="Y31" t="n">
-        <v>0.611801034317154</v>
+        <v>0.514153105072473</v>
       </c>
     </row>
     <row r="32">
@@ -3281,22 +3281,22 @@
         <v>176220.549942828</v>
       </c>
       <c r="T32" t="n">
-        <v>291391.006145506</v>
+        <v>219629.432294297</v>
       </c>
       <c r="U32" t="n">
-        <v>4573250.57969981</v>
+        <v>4501489.0058486</v>
       </c>
       <c r="V32" t="n">
-        <v>-1.7523644093836</v>
+        <v>-1.80840639602449</v>
       </c>
       <c r="W32" t="n">
-        <v>2.77081111658445</v>
+        <v>2.60916785638007</v>
       </c>
       <c r="X32" t="n">
-        <v>18098575.9924922</v>
+        <v>17832479.0875058</v>
       </c>
       <c r="Y32" t="n">
-        <v>0.611801034317154</v>
+        <v>0.514153105072473</v>
       </c>
     </row>
     <row r="33">
@@ -3358,22 +3358,22 @@
         <v>174574.888392839</v>
       </c>
       <c r="T33" t="n">
-        <v>305801.960928126</v>
+        <v>250167.863097608</v>
       </c>
       <c r="U33" t="n">
-        <v>4454856.40853514</v>
+        <v>4399222.31070462</v>
       </c>
       <c r="V33" t="n">
-        <v>-2.58884067473168</v>
+        <v>-2.27184149536096</v>
       </c>
       <c r="W33" t="n">
-        <v>-4.53933990586655</v>
+        <v>-4.57840782416044</v>
       </c>
       <c r="X33" t="n">
-        <v>18098575.9924922</v>
+        <v>17832479.0875058</v>
       </c>
       <c r="Y33" t="n">
-        <v>0.611801034317154</v>
+        <v>0.514153105072473</v>
       </c>
     </row>
     <row r="34">
@@ -3435,22 +3435,22 @@
         <v>174946.62805623</v>
       </c>
       <c r="T34" t="n">
-        <v>303023.26785299</v>
+        <v>238174.294704946</v>
       </c>
       <c r="U34" t="n">
-        <v>4327887.85713068</v>
+        <v>4263038.88398264</v>
       </c>
       <c r="V34" t="n">
-        <v>-2.85011546413021</v>
+        <v>-3.09562502423683</v>
       </c>
       <c r="W34" t="n">
-        <v>-1.98750304460818</v>
+        <v>-1.9399161552131</v>
       </c>
       <c r="X34" t="n">
-        <v>17759375.7333187</v>
+        <v>17522952.0152718</v>
       </c>
       <c r="Y34" t="n">
-        <v>-1.87418203130553</v>
+        <v>-1.73574897082532</v>
       </c>
     </row>
     <row r="35">
@@ -3512,22 +3512,22 @@
         <v>172404.785128273</v>
       </c>
       <c r="T35" t="n">
-        <v>294627.830546878</v>
+        <v>237421.712077554</v>
       </c>
       <c r="U35" t="n">
-        <v>4482948.85540643</v>
+        <v>4425742.73693711</v>
       </c>
       <c r="V35" t="n">
-        <v>3.58283309074814</v>
+        <v>3.81661667609437</v>
       </c>
       <c r="W35" t="n">
-        <v>-3.69232609461504</v>
+        <v>-3.46067009017354</v>
       </c>
       <c r="X35" t="n">
-        <v>17759375.7333187</v>
+        <v>17522952.0152718</v>
       </c>
       <c r="Y35" t="n">
-        <v>-1.87418203130553</v>
+        <v>-1.73574897082532</v>
       </c>
     </row>
     <row r="36">
@@ -3589,22 +3589,22 @@
         <v>170698.653409512</v>
       </c>
       <c r="T36" t="n">
-        <v>292467.013451496</v>
+        <v>236968.518827866</v>
       </c>
       <c r="U36" t="n">
-        <v>4464515.14847275</v>
+        <v>4409016.65384912</v>
       </c>
       <c r="V36" t="n">
-        <v>-0.41119601245165</v>
+        <v>-0.377927143129878</v>
       </c>
       <c r="W36" t="n">
-        <v>-2.37763991568102</v>
+        <v>-2.0542614205951</v>
       </c>
       <c r="X36" t="n">
-        <v>17759375.7333187</v>
+        <v>17522952.0152718</v>
       </c>
       <c r="Y36" t="n">
-        <v>-1.87418203130553</v>
+        <v>-1.73574897082532</v>
       </c>
     </row>
     <row r="37">
@@ -3666,22 +3666,22 @@
         <v>169828.232899947</v>
       </c>
       <c r="T37" t="n">
-        <v>299724.962428498</v>
+        <v>240854.830622614</v>
       </c>
       <c r="U37" t="n">
-        <v>4484023.87230884</v>
+        <v>4425153.74050296</v>
       </c>
       <c r="V37" t="n">
-        <v>0.436972956464622</v>
+        <v>0.366001943761111</v>
       </c>
       <c r="W37" t="n">
-        <v>0.654734094634891</v>
+        <v>0.589454861947814</v>
       </c>
       <c r="X37" t="n">
-        <v>17759375.7333187</v>
+        <v>17522952.0152718</v>
       </c>
       <c r="Y37" t="n">
-        <v>-1.87418203130553</v>
+        <v>-1.73574897082532</v>
       </c>
     </row>
     <row r="38">
@@ -3743,22 +3743,22 @@
         <v>168338.789577716</v>
       </c>
       <c r="T38" t="n">
-        <v>293497.62597663</v>
+        <v>237277.882732574</v>
       </c>
       <c r="U38" t="n">
-        <v>4506502.96440817</v>
+        <v>4450283.22116411</v>
       </c>
       <c r="V38" t="n">
-        <v>0.501315174483028</v>
+        <v>0.567878137908438</v>
       </c>
       <c r="W38" t="n">
-        <v>4.12707337097933</v>
+        <v>4.39227373423694</v>
       </c>
       <c r="X38" t="n">
-        <v>18181160.392964</v>
+        <v>17929261.6914465</v>
       </c>
       <c r="Y38" t="n">
-        <v>2.37499710563573</v>
+        <v>2.31872846436256</v>
       </c>
     </row>
     <row r="39">
@@ -3820,22 +3820,22 @@
         <v>168986.367091497</v>
       </c>
       <c r="T39" t="n">
-        <v>310593.729993313</v>
+        <v>249400.895340063</v>
       </c>
       <c r="U39" t="n">
-        <v>4680890.47630043</v>
+        <v>4619697.64164718</v>
       </c>
       <c r="V39" t="n">
-        <v>3.86968594649883</v>
+        <v>3.80682334277921</v>
       </c>
       <c r="W39" t="n">
-        <v>4.41543339615126</v>
+        <v>4.38242609746221</v>
       </c>
       <c r="X39" t="n">
-        <v>18181160.392964</v>
+        <v>17929261.6914465</v>
       </c>
       <c r="Y39" t="n">
-        <v>2.37499710563573</v>
+        <v>2.31872846436256</v>
       </c>
     </row>
     <row r="40">
@@ -3897,22 +3897,22 @@
         <v>170316.231419429</v>
       </c>
       <c r="T40" t="n">
-        <v>292139.526772953</v>
+        <v>219781.946630533</v>
       </c>
       <c r="U40" t="n">
-        <v>4461464.45170702</v>
+        <v>4389106.8715646</v>
       </c>
       <c r="V40" t="n">
-        <v>-4.68769832800775</v>
+        <v>-4.99146887891047</v>
       </c>
       <c r="W40" t="n">
-        <v>-0.0683320957434407</v>
+        <v>-0.45156967749586</v>
       </c>
       <c r="X40" t="n">
-        <v>18181160.392964</v>
+        <v>17929261.6914465</v>
       </c>
       <c r="Y40" t="n">
-        <v>2.37499710563573</v>
+        <v>2.31872846436256</v>
       </c>
     </row>
     <row r="41">
@@ -3974,22 +3974,22 @@
         <v>172328.382561511</v>
       </c>
       <c r="T41" t="n">
-        <v>340750.847043593</v>
+        <v>278622.303565847</v>
       </c>
       <c r="U41" t="n">
-        <v>4532302.50054839</v>
+        <v>4470173.95707064</v>
       </c>
       <c r="V41" t="n">
-        <v>1.58777570925764</v>
+        <v>1.84700641561604</v>
       </c>
       <c r="W41" t="n">
-        <v>1.07668089230494</v>
+        <v>1.0173706769917</v>
       </c>
       <c r="X41" t="n">
-        <v>18181160.392964</v>
+        <v>17929261.6914465</v>
       </c>
       <c r="Y41" t="n">
-        <v>2.37499710563573</v>
+        <v>2.31872846436256</v>
       </c>
     </row>
     <row r="42">
@@ -4051,22 +4051,22 @@
         <v>174162.17921548</v>
       </c>
       <c r="T42" t="n">
-        <v>310151.483563359</v>
+        <v>243194.395087331</v>
       </c>
       <c r="U42" t="n">
-        <v>4411982.16235685</v>
+        <v>4345025.07388082</v>
       </c>
       <c r="V42" t="n">
-        <v>-2.65472876483816</v>
+        <v>-2.79964234930648</v>
       </c>
       <c r="W42" t="n">
-        <v>-2.09743126317315</v>
+        <v>-2.36520109063442</v>
       </c>
       <c r="X42" t="n">
-        <v>17959549.4848559</v>
+        <v>17740852.2319601</v>
       </c>
       <c r="Y42" t="n">
-        <v>-1.21890409257824</v>
+        <v>-1.05084895702268</v>
       </c>
     </row>
     <row r="43">
@@ -4128,22 +4128,22 @@
         <v>176069.480173464</v>
       </c>
       <c r="T43" t="n">
-        <v>319531.994798751</v>
+        <v>258554.685223324</v>
       </c>
       <c r="U43" t="n">
-        <v>4529455.29177433</v>
+        <v>4468477.98219891</v>
       </c>
       <c r="V43" t="n">
-        <v>2.66259302722866</v>
+        <v>2.8412473166196</v>
       </c>
       <c r="W43" t="n">
-        <v>-3.23517897487275</v>
+        <v>-3.27336702915368</v>
       </c>
       <c r="X43" t="n">
-        <v>17959549.4848559</v>
+        <v>17740852.2319601</v>
       </c>
       <c r="Y43" t="n">
-        <v>-1.21890409257824</v>
+        <v>-1.05084895702268</v>
       </c>
     </row>
     <row r="44">
@@ -4205,22 +4205,22 @@
         <v>177189.6441332</v>
       </c>
       <c r="T44" t="n">
-        <v>305412.102357959</v>
+        <v>247028.933956566</v>
       </c>
       <c r="U44" t="n">
-        <v>4448322.3748026</v>
+        <v>4389939.2064012</v>
       </c>
       <c r="V44" t="n">
-        <v>-1.79122900537462</v>
+        <v>-1.75761805497486</v>
       </c>
       <c r="W44" t="n">
-        <v>-0.294568679111461</v>
+        <v>0.0189636493474164</v>
       </c>
       <c r="X44" t="n">
-        <v>17959549.4848559</v>
+        <v>17740852.2319601</v>
       </c>
       <c r="Y44" t="n">
-        <v>-1.21890409257824</v>
+        <v>-1.05084895702268</v>
       </c>
     </row>
     <row r="45">
@@ -4282,22 +4282,22 @@
         <v>177522.671094687</v>
       </c>
       <c r="T45" t="n">
-        <v>367467.191322159</v>
+        <v>335087.504879152</v>
       </c>
       <c r="U45" t="n">
-        <v>4569789.65592217</v>
+        <v>4537409.96947916</v>
       </c>
       <c r="V45" t="n">
-        <v>2.73063125567565</v>
+        <v>3.35928941482662</v>
       </c>
       <c r="W45" t="n">
-        <v>0.827110621350804</v>
+        <v>1.50410281689763</v>
       </c>
       <c r="X45" t="n">
-        <v>17959549.4848559</v>
+        <v>17740852.2319601</v>
       </c>
       <c r="Y45" t="n">
-        <v>-1.21890409257824</v>
+        <v>-1.05084895702268</v>
       </c>
     </row>
     <row r="46">
@@ -4359,22 +4359,22 @@
         <v>179786.370809749</v>
       </c>
       <c r="T46" t="n">
-        <v>296563.57049879</v>
+        <v>259517.126632385</v>
       </c>
       <c r="U46" t="n">
-        <v>4451191.00398672</v>
+        <v>4414144.56012031</v>
       </c>
       <c r="V46" t="n">
-        <v>-2.59527595065025</v>
+        <v>-2.71664694590068</v>
       </c>
       <c r="W46" t="n">
-        <v>0.888689939963972</v>
+        <v>1.59077301198998</v>
       </c>
       <c r="X46" t="n">
-        <v>18313699.1484691</v>
+        <v>18194180.6788699</v>
       </c>
       <c r="Y46" t="n">
-        <v>1.97192955152797</v>
+        <v>2.55527998870938</v>
       </c>
     </row>
     <row r="47">
@@ -4436,22 +4436,22 @@
         <v>180280.098706662</v>
       </c>
       <c r="T47" t="n">
-        <v>313737.304652425</v>
+        <v>287694.356884507</v>
       </c>
       <c r="U47" t="n">
-        <v>4662317.91204745</v>
+        <v>4636274.96427953</v>
       </c>
       <c r="V47" t="n">
-        <v>4.74315543573925</v>
+        <v>5.03224126744876</v>
       </c>
       <c r="W47" t="n">
-        <v>2.93330238879718</v>
+        <v>3.75512607982134</v>
       </c>
       <c r="X47" t="n">
-        <v>18313699.1484691</v>
+        <v>18194180.6788699</v>
       </c>
       <c r="Y47" t="n">
-        <v>1.97192955152797</v>
+        <v>2.55527998870938</v>
       </c>
     </row>
     <row r="48">
@@ -4513,22 +4513,22 @@
         <v>181721.66453725</v>
       </c>
       <c r="T48" t="n">
-        <v>291440.178688865</v>
+        <v>259923.405725136</v>
       </c>
       <c r="U48" t="n">
-        <v>4563279.65801842</v>
+        <v>4531762.88505469</v>
       </c>
       <c r="V48" t="n">
-        <v>-2.12422781752223</v>
+        <v>-2.25422521377753</v>
       </c>
       <c r="W48" t="n">
-        <v>2.58428399584961</v>
+        <v>3.23065245292428</v>
       </c>
       <c r="X48" t="n">
-        <v>18313699.1484691</v>
+        <v>18194180.6788699</v>
       </c>
       <c r="Y48" t="n">
-        <v>1.97192955152797</v>
+        <v>2.55527998870938</v>
       </c>
     </row>
     <row r="49">
@@ -4590,22 +4590,22 @@
         <v>184111.068301513</v>
       </c>
       <c r="T49" t="n">
-        <v>335897.016249502</v>
+        <v>310984.711248312</v>
       </c>
       <c r="U49" t="n">
-        <v>4636910.57441652</v>
+        <v>4611998.26941533</v>
       </c>
       <c r="V49" t="n">
-        <v>1.61355257437985</v>
+        <v>1.77051152930475</v>
       </c>
       <c r="W49" t="n">
-        <v>1.46879667442398</v>
+        <v>1.64385189872394</v>
       </c>
       <c r="X49" t="n">
-        <v>18313699.1484691</v>
+        <v>18194180.6788699</v>
       </c>
       <c r="Y49" t="n">
-        <v>1.97192955152797</v>
+        <v>2.55527998870938</v>
       </c>
     </row>
     <row r="50">
@@ -4667,22 +4667,22 @@
         <v>189728.752330248</v>
       </c>
       <c r="T50" t="n">
-        <v>287320.352746826</v>
+        <v>269786.864586886</v>
       </c>
       <c r="U50" t="n">
-        <v>4613976.90946685</v>
+        <v>4596443.42130691</v>
       </c>
       <c r="V50" t="n">
-        <v>-0.494589330150319</v>
+        <v>-0.337269166200221</v>
       </c>
       <c r="W50" t="n">
-        <v>3.65713143593099</v>
+        <v>4.12987972422967</v>
       </c>
       <c r="X50" t="n">
-        <v>19201186.8351446</v>
+        <v>19133855.8442888</v>
       </c>
       <c r="Y50" t="n">
-        <v>4.84603181192715</v>
+        <v>5.16470173625488</v>
       </c>
     </row>
     <row r="51">
@@ -4744,22 +4744,22 @@
         <v>192666.253167523</v>
       </c>
       <c r="T51" t="n">
-        <v>339711.86811528</v>
+        <v>329222.653902289</v>
       </c>
       <c r="U51" t="n">
-        <v>4846250.56608984</v>
+        <v>4835761.35187685</v>
       </c>
       <c r="V51" t="n">
-        <v>5.03413131839514</v>
+        <v>5.20658928293506</v>
       </c>
       <c r="W51" t="n">
-        <v>3.9450903501691</v>
+        <v>4.30272986684938</v>
       </c>
       <c r="X51" t="n">
-        <v>19201186.8351446</v>
+        <v>19133855.8442888</v>
       </c>
       <c r="Y51" t="n">
-        <v>4.84603181192715</v>
+        <v>5.16470173625488</v>
       </c>
     </row>
     <row r="52">
@@ -4821,22 +4821,22 @@
         <v>195204.013144137</v>
       </c>
       <c r="T52" t="n">
-        <v>289026.882847885</v>
+        <v>262046.123666926</v>
       </c>
       <c r="U52" t="n">
-        <v>4804980.60050114</v>
+        <v>4777999.84132018</v>
       </c>
       <c r="V52" t="n">
-        <v>-0.851585468516075</v>
+        <v>-1.19446569740769</v>
       </c>
       <c r="W52" t="n">
-        <v>5.29664979129685</v>
+        <v>5.4335798785404</v>
       </c>
       <c r="X52" t="n">
-        <v>19201186.8351446</v>
+        <v>19133855.8442888</v>
       </c>
       <c r="Y52" t="n">
-        <v>4.84603181192715</v>
+        <v>5.16470173625488</v>
       </c>
     </row>
     <row r="53">
@@ -4898,22 +4898,22 @@
         <v>197342.032260087</v>
       </c>
       <c r="T53" t="n">
-        <v>338673.257020824</v>
+        <v>326345.72771897</v>
       </c>
       <c r="U53" t="n">
-        <v>4935978.75908672</v>
+        <v>4923651.22978487</v>
       </c>
       <c r="V53" t="n">
-        <v>2.72629942713861</v>
+        <v>3.04837574930612</v>
       </c>
       <c r="W53" t="n">
-        <v>6.44972940216412</v>
+        <v>6.75743879689365</v>
       </c>
       <c r="X53" t="n">
-        <v>19201186.8351446</v>
+        <v>19133855.8442888</v>
       </c>
       <c r="Y53" t="n">
-        <v>4.84603181192715</v>
+        <v>5.16470173625488</v>
       </c>
     </row>
     <row r="54">
@@ -4975,22 +4975,22 @@
         <v>204417.269806214</v>
       </c>
       <c r="T54" t="n">
-        <v>293210.434554792</v>
+        <v>288546.702249115</v>
       </c>
       <c r="U54" t="n">
-        <v>4937656.847332</v>
+        <v>4932993.11502633</v>
       </c>
       <c r="V54" t="n">
-        <v>0.0339970718510663</v>
+        <v>0.189734910241896</v>
       </c>
       <c r="W54" t="n">
-        <v>7.01520497861697</v>
+        <v>7.32195880317671</v>
       </c>
       <c r="X54" t="n">
-        <v>20004229.4650259</v>
+        <v>19953355.8972754</v>
       </c>
       <c r="Y54" t="n">
-        <v>4.18225517399522</v>
+        <v>4.28298435848828</v>
       </c>
     </row>
     <row r="55">
@@ -5052,22 +5052,22 @@
         <v>202315.57313147</v>
       </c>
       <c r="T55" t="n">
-        <v>318348.831397347</v>
+        <v>318508.28630051</v>
       </c>
       <c r="U55" t="n">
-        <v>5115904.67789982</v>
+        <v>5116064.13280298</v>
       </c>
       <c r="V55" t="n">
-        <v>3.60996796818974</v>
+        <v>3.71115494199663</v>
       </c>
       <c r="W55" t="n">
-        <v>5.56418014571512</v>
+        <v>5.79645603928202</v>
       </c>
       <c r="X55" t="n">
-        <v>20004229.4650259</v>
+        <v>19953355.8972754</v>
       </c>
       <c r="Y55" t="n">
-        <v>4.18225517399522</v>
+        <v>4.28298435848828</v>
       </c>
     </row>
     <row r="56">
@@ -5129,22 +5129,22 @@
         <v>196373.901526694</v>
       </c>
       <c r="T56" t="n">
-        <v>280143.601340327</v>
+        <v>260682.851654286</v>
       </c>
       <c r="U56" t="n">
-        <v>5010812.09322523</v>
+        <v>4991351.34353918</v>
       </c>
       <c r="V56" t="n">
-        <v>-2.05423265856732</v>
+        <v>-2.43767056132402</v>
       </c>
       <c r="W56" t="n">
-        <v>4.28371121212472</v>
+        <v>4.46528901851227</v>
       </c>
       <c r="X56" t="n">
-        <v>20004229.4650259</v>
+        <v>19953355.8972754</v>
       </c>
       <c r="Y56" t="n">
-        <v>4.18225517399522</v>
+        <v>4.28298435848828</v>
       </c>
     </row>
     <row r="57">
@@ -5206,22 +5206,22 @@
         <v>186592.254991886</v>
       </c>
       <c r="T57" t="n">
-        <v>314802.89633086</v>
+        <v>287894.355668935</v>
       </c>
       <c r="U57" t="n">
-        <v>4939855.84656883</v>
+        <v>4912947.3059069</v>
       </c>
       <c r="V57" t="n">
-        <v>-1.41606281249966</v>
+        <v>-1.57079781077259</v>
       </c>
       <c r="W57" t="n">
-        <v>0.0785474912136879</v>
+        <v>-0.217398092968401</v>
       </c>
       <c r="X57" t="n">
-        <v>20004229.4650259</v>
+        <v>19953355.8972754</v>
       </c>
       <c r="Y57" t="n">
-        <v>4.18225517399522</v>
+        <v>4.28298435848828</v>
       </c>
     </row>
     <row r="58">
@@ -5283,22 +5283,22 @@
         <v>174576.656403357</v>
       </c>
       <c r="T58" t="n">
-        <v>93666.240479178</v>
+        <v>7652.00714523399</v>
       </c>
       <c r="U58" t="n">
-        <v>4332261.26012451</v>
+        <v>4246247.02679056</v>
       </c>
       <c r="V58" t="n">
-        <v>-12.2998444755498</v>
+        <v>-13.570271317886</v>
       </c>
       <c r="W58" t="n">
-        <v>-12.2607869668913</v>
+        <v>-13.9214888855992</v>
       </c>
       <c r="X58" t="n">
-        <v>18943088.2721304</v>
+        <v>18760880.2397218</v>
       </c>
       <c r="Y58" t="n">
-        <v>-5.30458418681248</v>
+        <v>-5.97631628329983</v>
       </c>
     </row>
     <row r="59">
@@ -5360,22 +5360,22 @@
         <v>166428.8512505</v>
       </c>
       <c r="T59" t="n">
-        <v>306608.978794906</v>
+        <v>264529.039928249</v>
       </c>
       <c r="U59" t="n">
-        <v>4584889.66609499</v>
+        <v>4542809.72722833</v>
       </c>
       <c r="V59" t="n">
-        <v>5.83132897121763</v>
+        <v>6.98411323144135</v>
       </c>
       <c r="W59" t="n">
-        <v>-10.3796893264795</v>
+        <v>-11.2049886532712</v>
       </c>
       <c r="X59" t="n">
-        <v>18943088.2721304</v>
+        <v>18760880.2397218</v>
       </c>
       <c r="Y59" t="n">
-        <v>-5.30458418681248</v>
+        <v>-5.97631628329983</v>
       </c>
     </row>
     <row r="60">
@@ -5437,22 +5437,22 @@
         <v>163754.862409625</v>
       </c>
       <c r="T60" t="n">
-        <v>356927.565351153</v>
+        <v>325935.605279838</v>
       </c>
       <c r="U60" t="n">
-        <v>4934509.36370529</v>
+        <v>4903517.40363398</v>
       </c>
       <c r="V60" t="n">
-        <v>7.62547679600063</v>
+        <v>7.94018895934965</v>
       </c>
       <c r="W60" t="n">
-        <v>-1.52276174201581</v>
+        <v>-1.75972264542952</v>
       </c>
       <c r="X60" t="n">
-        <v>18943088.2721304</v>
+        <v>18760880.2397218</v>
       </c>
       <c r="Y60" t="n">
-        <v>-5.30458418681248</v>
+        <v>-5.97631628329983</v>
       </c>
     </row>
     <row r="61">
@@ -5514,22 +5514,22 @@
         <v>166554.689880733</v>
       </c>
       <c r="T61" t="n">
-        <v>354837.496692812</v>
+        <v>331715.596556057</v>
       </c>
       <c r="U61" t="n">
-        <v>5091427.98220564</v>
+        <v>5068306.08206889</v>
       </c>
       <c r="V61" t="n">
-        <v>3.18002473872141</v>
+        <v>3.36062187344923</v>
       </c>
       <c r="W61" t="n">
-        <v>3.06835139211797</v>
+        <v>3.16223168066947</v>
       </c>
       <c r="X61" t="n">
-        <v>18943088.2721304</v>
+        <v>18760880.2397218</v>
       </c>
       <c r="Y61" t="n">
-        <v>-5.30458418681248</v>
+        <v>-5.97631628329983</v>
       </c>
     </row>
     <row r="62">
@@ -5591,22 +5591,22 @@
         <v>161945.241946783</v>
       </c>
       <c r="T62" t="n">
-        <v>369982.210475505</v>
+        <v>335569.457181876</v>
       </c>
       <c r="U62" t="n">
-        <v>5155184.01601041</v>
+        <v>5120771.26271678</v>
       </c>
       <c r="V62" t="n">
-        <v>1.25222303109449</v>
+        <v>1.035162040302</v>
       </c>
       <c r="W62" t="n">
-        <v>18.995224583068</v>
+        <v>20.5952275128753</v>
       </c>
       <c r="X62" t="n">
-        <v>21099342.179223</v>
+        <v>21039989.6132708</v>
       </c>
       <c r="Y62" t="n">
-        <v>11.3828002916764</v>
+        <v>12.1482006410527</v>
       </c>
     </row>
     <row r="63">
@@ -5668,22 +5668,22 @@
         <v>170379.658267379</v>
       </c>
       <c r="T63" t="n">
-        <v>372207.408387963</v>
+        <v>354408.807153539</v>
       </c>
       <c r="U63" t="n">
-        <v>5355991.56740867</v>
+        <v>5338192.96617425</v>
       </c>
       <c r="V63" t="n">
-        <v>3.89525477217915</v>
+        <v>4.24587805826179</v>
       </c>
       <c r="W63" t="n">
-        <v>16.8183305918122</v>
+        <v>17.508618821929</v>
       </c>
       <c r="X63" t="n">
-        <v>21099342.179223</v>
+        <v>21039989.6132708</v>
       </c>
       <c r="Y63" t="n">
-        <v>11.3828002916764</v>
+        <v>12.1482006410527</v>
       </c>
     </row>
     <row r="64">
@@ -5745,22 +5745,22 @@
         <v>178974.84712548</v>
       </c>
       <c r="T64" t="n">
-        <v>371676.580599354</v>
+        <v>366464.59881831</v>
       </c>
       <c r="U64" t="n">
-        <v>5240190.00316889</v>
+        <v>5234978.02138785</v>
       </c>
       <c r="V64" t="n">
-        <v>-2.16209384914715</v>
+        <v>-1.93351842918438</v>
       </c>
       <c r="W64" t="n">
-        <v>6.19475244513605</v>
+        <v>6.75965007299103</v>
       </c>
       <c r="X64" t="n">
-        <v>21099342.179223</v>
+        <v>21039989.6132708</v>
       </c>
       <c r="Y64" t="n">
-        <v>11.3828002916764</v>
+        <v>12.1482006410527</v>
       </c>
     </row>
     <row r="65">
@@ -5822,22 +5822,22 @@
         <v>187730.808521086</v>
       </c>
       <c r="T65" t="n">
-        <v>348762.143016394</v>
+        <v>346832.91337326</v>
       </c>
       <c r="U65" t="n">
-        <v>5347976.59263502</v>
+        <v>5346047.36299189</v>
       </c>
       <c r="V65" t="n">
-        <v>2.0569213979064</v>
+        <v>2.12167732415039</v>
       </c>
       <c r="W65" t="n">
-        <v>5.03883412131153</v>
+        <v>5.47996266258701</v>
       </c>
       <c r="X65" t="n">
-        <v>21099342.179223</v>
+        <v>21039989.6132708</v>
       </c>
       <c r="Y65" t="n">
-        <v>11.3828002916764</v>
+        <v>12.1482006410527</v>
       </c>
     </row>
     <row r="66">
@@ -5899,22 +5899,22 @@
         <v>199663.684975644</v>
       </c>
       <c r="T66" t="n">
-        <v>342278.945138961</v>
+        <v>349399.137504528</v>
       </c>
       <c r="U66" t="n">
-        <v>5491512.95202606</v>
+        <v>5498633.14439163</v>
       </c>
       <c r="V66" t="n">
-        <v>2.68393768941898</v>
+        <v>2.85417937850712</v>
       </c>
       <c r="W66" t="n">
-        <v>6.52409176803611</v>
+        <v>7.37900332369803</v>
       </c>
       <c r="X66" t="n">
-        <v>23068581.5878245</v>
+        <v>23172765.115995</v>
       </c>
       <c r="Y66" t="n">
-        <v>9.33317916679234</v>
+        <v>10.1367707015359</v>
       </c>
     </row>
     <row r="67">
@@ -5976,22 +5976,22 @@
         <v>199732.463820849</v>
       </c>
       <c r="T67" t="n">
-        <v>381170.199601206</v>
+        <v>405629.155865216</v>
       </c>
       <c r="U67" t="n">
-        <v>5837712.01146707</v>
+        <v>5862170.96773108</v>
       </c>
       <c r="V67" t="n">
-        <v>6.30425644927747</v>
+        <v>6.61142167140658</v>
       </c>
       <c r="W67" t="n">
-        <v>8.99404784334756</v>
+        <v>9.81564369960107</v>
       </c>
       <c r="X67" t="n">
-        <v>23068581.5878245</v>
+        <v>23172765.115995</v>
       </c>
       <c r="Y67" t="n">
-        <v>9.33317916679234</v>
+        <v>10.1367707015359</v>
       </c>
     </row>
     <row r="68">
@@ -6053,22 +6053,22 @@
         <v>190953.287578148</v>
       </c>
       <c r="T68" t="n">
-        <v>364275.879995934</v>
+        <v>391805.093962095</v>
       </c>
       <c r="U68" t="n">
-        <v>5720384.11805237</v>
+        <v>5747913.33201853</v>
       </c>
       <c r="V68" t="n">
-        <v>-2.00982667840123</v>
+        <v>-1.9490669300075</v>
       </c>
       <c r="W68" t="n">
-        <v>9.16367754972805</v>
+        <v>9.79823236191357</v>
       </c>
       <c r="X68" t="n">
-        <v>23068581.5878245</v>
+        <v>23172765.115995</v>
       </c>
       <c r="Y68" t="n">
-        <v>9.33317916679234</v>
+        <v>10.1367707015359</v>
       </c>
     </row>
     <row r="69">
@@ -6130,22 +6130,22 @@
         <v>173326.156247541</v>
       </c>
       <c r="T69" t="n">
-        <v>398522.334964433</v>
+        <v>443597.500539226</v>
       </c>
       <c r="U69" t="n">
-        <v>6018972.50627897</v>
+        <v>6064047.67185376</v>
       </c>
       <c r="V69" t="n">
-        <v>5.21972619433564</v>
+        <v>5.49998445651945</v>
       </c>
       <c r="W69" t="n">
-        <v>12.5467249532843</v>
+        <v>13.4304891092481</v>
       </c>
       <c r="X69" t="n">
-        <v>23068581.5878245</v>
+        <v>23172765.115995</v>
       </c>
       <c r="Y69" t="n">
-        <v>9.33317916679234</v>
+        <v>10.1367707015359</v>
       </c>
     </row>
     <row r="70">
@@ -6207,22 +6207,22 @@
         <v>218431.327059074</v>
       </c>
       <c r="T70" t="n">
-        <v>349469.179414627</v>
+        <v>412742.591113907</v>
       </c>
       <c r="U70" t="n">
-        <v>6110736.47143148</v>
+        <v>6174009.88313076</v>
       </c>
       <c r="V70" t="n">
-        <v>1.52457857311657</v>
+        <v>1.81334674836714</v>
       </c>
       <c r="W70" t="n">
-        <v>11.2760094497629</v>
+        <v>12.2826295372693</v>
       </c>
       <c r="X70" t="n">
-        <v>25279048.8557045</v>
+        <v>25508162.7908763</v>
       </c>
       <c r="Y70" t="n">
-        <v>9.58215510331454</v>
+        <v>10.0782002630721</v>
       </c>
     </row>
     <row r="71">
@@ -6284,22 +6284,22 @@
         <v>210806.110485631</v>
       </c>
       <c r="T71" t="n">
-        <v>417358.6004381</v>
+        <v>494524.575229555</v>
       </c>
       <c r="U71" t="n">
-        <v>6481631.24103243</v>
+        <v>6558797.21582388</v>
       </c>
       <c r="V71" t="n">
-        <v>6.06955923127981</v>
+        <v>6.23237312503304</v>
       </c>
       <c r="W71" t="n">
-        <v>11.0303356571975</v>
+        <v>11.8834174562197</v>
       </c>
       <c r="X71" t="n">
-        <v>25279048.8557045</v>
+        <v>25508162.7908763</v>
       </c>
       <c r="Y71" t="n">
-        <v>9.58215510331454</v>
+        <v>10.0782002630721</v>
       </c>
     </row>
     <row r="72">
@@ -6361,22 +6361,22 @@
         <v>196509.974807126</v>
       </c>
       <c r="T72" t="n">
-        <v>386878.705866908</v>
+        <v>438068.086860078</v>
       </c>
       <c r="U72" t="n">
-        <v>6308618.70462523</v>
+        <v>6359808.0856184</v>
       </c>
       <c r="V72" t="n">
-        <v>-2.66927460038039</v>
+        <v>-3.03392716160514</v>
       </c>
       <c r="W72" t="n">
-        <v>10.2831308952926</v>
+        <v>10.6455111316889</v>
       </c>
       <c r="X72" t="n">
-        <v>25279048.8557045</v>
+        <v>25508162.7908763</v>
       </c>
       <c r="Y72" t="n">
-        <v>9.58215510331454</v>
+        <v>10.0782002630721</v>
       </c>
     </row>
     <row r="73">
@@ -6438,22 +6438,22 @@
         <v>213596.905371914</v>
       </c>
       <c r="T73" t="n">
-        <v>451992.24940533</v>
+        <v>489477.417093256</v>
       </c>
       <c r="U73" t="n">
-        <v>6378062.43861534</v>
+        <v>6415547.60630327</v>
       </c>
       <c r="V73" t="n">
-        <v>1.10077557769026</v>
+        <v>0.876434004524684</v>
       </c>
       <c r="W73" t="n">
-        <v>5.96596731355347</v>
+        <v>5.79645730822649</v>
       </c>
       <c r="X73" t="n">
-        <v>25279048.8557045</v>
+        <v>25508162.7908763</v>
       </c>
       <c r="Y73" t="n">
-        <v>9.58215510331454</v>
+        <v>10.0782002630721</v>
       </c>
     </row>
     <row r="74">
@@ -6515,22 +6515,22 @@
         <v>206691.008306889</v>
       </c>
       <c r="T74" t="n">
-        <v>468185.763396828</v>
+        <v>467892.665035613</v>
       </c>
       <c r="U74" t="n">
-        <v>6551107.71320083</v>
+        <v>6550814.61483961</v>
       </c>
       <c r="V74" t="n">
-        <v>2.71313233840113</v>
+        <v>2.10842498313701</v>
       </c>
       <c r="W74" t="n">
-        <v>7.20651665847726</v>
+        <v>6.10307950329659</v>
       </c>
       <c r="X74" t="n">
-        <v>27207068.5433433</v>
+        <v>27207274.8436116</v>
       </c>
       <c r="Y74" t="n">
-        <v>7.62694711594653</v>
+        <v>6.66105225478259</v>
       </c>
     </row>
     <row r="75">
@@ -6592,22 +6592,22 @@
         <v>231646.552017198</v>
       </c>
       <c r="T75" t="n">
-        <v>534126.868598056</v>
+        <v>530429.245959462</v>
       </c>
       <c r="U75" t="n">
-        <v>6957927.14712245</v>
+        <v>6954229.52448385</v>
       </c>
       <c r="V75" t="n">
-        <v>6.20993352165242</v>
+        <v>6.15824036189909</v>
       </c>
       <c r="W75" t="n">
-        <v>7.34839561798571</v>
+        <v>6.02903696589283</v>
       </c>
       <c r="X75" t="n">
-        <v>27207068.5433433</v>
+        <v>27207274.8436116</v>
       </c>
       <c r="Y75" t="n">
-        <v>7.62694711594653</v>
+        <v>6.66105225478259</v>
       </c>
     </row>
     <row r="76">
@@ -6669,22 +6669,22 @@
         <v>220286.182123275</v>
       </c>
       <c r="T76" t="n">
-        <v>487884.875635688</v>
+        <v>474127.897514206</v>
       </c>
       <c r="U76" t="n">
-        <v>6778727.07707326</v>
+        <v>6764970.09895177</v>
       </c>
       <c r="V76" t="n">
-        <v>-2.57548068929264</v>
+        <v>-2.72150099253626</v>
       </c>
       <c r="W76" t="n">
-        <v>7.45184317611975</v>
+        <v>6.37066414393195</v>
       </c>
       <c r="X76" t="n">
-        <v>27207068.5433433</v>
+        <v>27207274.8436116</v>
       </c>
       <c r="Y76" t="n">
-        <v>7.62694711594653</v>
+        <v>6.66105225478259</v>
       </c>
     </row>
     <row r="77">
@@ -6746,22 +6746,22 @@
         <v>222709.341859818</v>
       </c>
       <c r="T77" t="n">
-        <v>509597.898344325</v>
+        <v>527551.897733862</v>
       </c>
       <c r="U77" t="n">
-        <v>6919306.60594681</v>
+        <v>6937260.60533634</v>
       </c>
       <c r="V77" t="n">
-        <v>2.07383373419786</v>
+        <v>2.54680366453158</v>
       </c>
       <c r="W77" t="n">
-        <v>8.48602804598707</v>
+        <v>8.13201040735</v>
       </c>
       <c r="X77" t="n">
-        <v>27207068.5433433</v>
+        <v>27207274.8436116</v>
       </c>
       <c r="Y77" t="n">
-        <v>7.62694711594653</v>
+        <v>6.66105225478259</v>
       </c>
     </row>
     <row r="78">
@@ -6823,22 +6823,22 @@
         <v>214684.055204205</v>
       </c>
       <c r="T78" t="n">
-        <v>540751.434087388</v>
+        <v>546947.546288576</v>
       </c>
       <c r="U78" t="n">
-        <v>7151656.85414286</v>
+        <v>7157852.96634404</v>
       </c>
       <c r="V78" t="n">
-        <v>3.35799902256618</v>
+        <v>3.17981943532602</v>
       </c>
       <c r="W78" t="n">
-        <v>9.1671388600723</v>
+        <v>9.26660861580942</v>
       </c>
       <c r="X78" t="n">
-        <v>29157477.1692881</v>
+        <v>29199249.987527</v>
       </c>
       <c r="Y78" t="n">
-        <v>7.1687569825377</v>
+        <v>7.32147984450973</v>
       </c>
     </row>
     <row r="79">
@@ -6900,22 +6900,22 @@
         <v>230293.058120855</v>
       </c>
       <c r="T79" t="n">
-        <v>546223.39259323</v>
+        <v>578694.233885731</v>
       </c>
       <c r="U79" t="n">
-        <v>7493332.23486494</v>
+        <v>7525803.07615744</v>
       </c>
       <c r="V79" t="n">
-        <v>4.77756955752366</v>
+        <v>5.14050947321052</v>
       </c>
       <c r="W79" t="n">
-        <v>7.6948935569686</v>
+        <v>8.21907803964827</v>
       </c>
       <c r="X79" t="n">
-        <v>29157477.1692881</v>
+        <v>29199249.987527</v>
       </c>
       <c r="Y79" t="n">
-        <v>7.1687569825377</v>
+        <v>7.32147984450973</v>
       </c>
     </row>
     <row r="80">
@@ -6977,22 +6977,22 @@
         <v>253511.212467653</v>
       </c>
       <c r="T80" t="n">
-        <v>470661.243065634</v>
+        <v>483050.24096678</v>
       </c>
       <c r="U80" t="n">
-        <v>7231445.17150598</v>
+        <v>7243834.16940712</v>
       </c>
       <c r="V80" t="n">
-        <v>-3.4949346318912</v>
+        <v>-3.74669525493729</v>
       </c>
       <c r="W80" t="n">
-        <v>6.67851189884731</v>
+        <v>7.07858369587693</v>
       </c>
       <c r="X80" t="n">
-        <v>29157477.1692881</v>
+        <v>29199249.987527</v>
       </c>
       <c r="Y80" t="n">
-        <v>7.1687569825377</v>
+        <v>7.32147984450973</v>
       </c>
     </row>
     <row r="81">
@@ -7054,22 +7054,22 @@
         <v>275478.748244096</v>
       </c>
       <c r="T81" t="n">
-        <v>480592.332259601</v>
+        <v>471309.199103654</v>
       </c>
       <c r="U81" t="n">
-        <v>7281042.90877431</v>
+        <v>7271759.77561836</v>
       </c>
       <c r="V81" t="n">
-        <v>0.685862038528069</v>
+        <v>0.385508634766583</v>
       </c>
       <c r="W81" t="n">
-        <v>5.22792706593762</v>
+        <v>4.821776048383</v>
       </c>
       <c r="X81" t="n">
-        <v>29157477.1692881</v>
+        <v>29199249.987527</v>
       </c>
       <c r="Y81" t="n">
-        <v>7.1687569825377</v>
+        <v>7.32147984450973</v>
       </c>
     </row>
     <row r="82">
@@ -7131,22 +7131,22 @@
         <v>301001.104762242</v>
       </c>
       <c r="T82" t="n">
-        <v>607148.546464222</v>
+        <v>603141.970682909</v>
       </c>
       <c r="U82" t="n">
-        <v>7717653.05772547</v>
+        <v>7713646.48194416</v>
       </c>
       <c r="V82" t="n">
-        <v>5.99653311237886</v>
+        <v>6.0767506072933</v>
       </c>
       <c r="W82" t="n">
-        <v>7.91419687949293</v>
+        <v>7.76480766248532</v>
       </c>
       <c r="X82" t="n">
-        <v>31350251.405438</v>
+        <v>31185550.5410978</v>
       </c>
       <c r="Y82" t="n">
-        <v>7.52045255293772</v>
+        <v>6.80257388261467</v>
       </c>
     </row>
     <row r="83">
@@ -7208,22 +7208,22 @@
         <v>340874.031723638</v>
       </c>
       <c r="T83" t="n">
-        <v>623013.73041612</v>
+        <v>588217.595036016</v>
       </c>
       <c r="U83" t="n">
-        <v>7938747.4691896</v>
+        <v>7903951.3338095</v>
       </c>
       <c r="V83" t="n">
-        <v>2.86478816565629</v>
+        <v>2.46711918041356</v>
       </c>
       <c r="W83" t="n">
-        <v>5.94415435435037</v>
+        <v>5.02468977496998</v>
       </c>
       <c r="X83" t="n">
-        <v>31350251.405438</v>
+        <v>31185550.5410978</v>
       </c>
       <c r="Y83" t="n">
-        <v>7.52045255293772</v>
+        <v>6.80257388261467</v>
       </c>
     </row>
     <row r="84">
@@ -7285,22 +7285,22 @@
         <v>324771.107962065</v>
       </c>
       <c r="T84" t="n">
-        <v>608749.500606898</v>
+        <v>548924.484583371</v>
       </c>
       <c r="U84" t="n">
-        <v>7722282.49612842</v>
+        <v>7662457.48010489</v>
       </c>
       <c r="V84" t="n">
-        <v>-2.72668924035295</v>
+        <v>-3.05535603023778</v>
       </c>
       <c r="W84" t="n">
-        <v>6.78754125878578</v>
+        <v>5.77902946019579</v>
       </c>
       <c r="X84" t="n">
-        <v>31350251.405438</v>
+        <v>31185550.5410978</v>
       </c>
       <c r="Y84" t="n">
-        <v>7.52045255293772</v>
+        <v>6.80257388261467</v>
       </c>
     </row>
     <row r="85">
@@ -7362,22 +7362,22 @@
         <v>313951.814944712</v>
       </c>
       <c r="T85" t="n">
-        <v>612789.61647067</v>
+        <v>546716.479315421</v>
       </c>
       <c r="U85" t="n">
-        <v>7971568.38239455</v>
+        <v>7905495.2452393</v>
       </c>
       <c r="V85" t="n">
-        <v>3.22813735953209</v>
+        <v>3.17179920104536</v>
       </c>
       <c r="W85" t="n">
-        <v>9.48388139270672</v>
+        <v>8.71502207410375</v>
       </c>
       <c r="X85" t="n">
-        <v>31350251.405438</v>
+        <v>31185550.5410978</v>
       </c>
       <c r="Y85" t="n">
-        <v>7.52045255293772</v>
+        <v>6.80257388261467</v>
       </c>
     </row>
     <row r="86">
@@ -7439,22 +7439,22 @@
         <v>280057.685354488</v>
       </c>
       <c r="T86" t="n">
-        <v>600985.859907447</v>
+        <v>521385.541225889</v>
       </c>
       <c r="U86" t="n">
-        <v>8131899.35985155</v>
+        <v>8052299.04117</v>
       </c>
       <c r="V86" t="n">
-        <v>2.01128522978116</v>
+        <v>1.85698417843086</v>
       </c>
       <c r="W86" t="n">
-        <v>5.36751651088299</v>
+        <v>4.39030437833187</v>
       </c>
       <c r="X86" t="n">
-        <v>33446104.7414181</v>
+        <v>33256250.1323107</v>
       </c>
       <c r="Y86" t="n">
-        <v>6.68528398345308</v>
+        <v>6.63993277426351</v>
       </c>
     </row>
     <row r="87">
@@ -7516,22 +7516,22 @@
         <v>284653.46074543</v>
       </c>
       <c r="T87" t="n">
-        <v>701757.83974922</v>
+        <v>659418.989103094</v>
       </c>
       <c r="U87" t="n">
-        <v>8523194.6261713</v>
+        <v>8480855.77552517</v>
       </c>
       <c r="V87" t="n">
-        <v>4.81185574248041</v>
+        <v>5.32216615607592</v>
       </c>
       <c r="W87" t="n">
-        <v>7.36195677277735</v>
+        <v>7.29893716890611</v>
       </c>
       <c r="X87" t="n">
-        <v>33446104.7414181</v>
+        <v>33256250.1323107</v>
       </c>
       <c r="Y87" t="n">
-        <v>6.68528398345308</v>
+        <v>6.63993277426351</v>
       </c>
     </row>
     <row r="88">
@@ -7593,22 +7593,22 @@
         <v>290295.255087058</v>
       </c>
       <c r="T88" t="n">
-        <v>626452.59372185</v>
+        <v>577687.458823942</v>
       </c>
       <c r="U88" t="n">
-        <v>8325796.09518067</v>
+        <v>8277030.96028277</v>
       </c>
       <c r="V88" t="n">
-        <v>-2.3160157622647</v>
+        <v>-2.40335198047609</v>
       </c>
       <c r="W88" t="n">
-        <v>7.815223016703</v>
+        <v>8.02057932162857</v>
       </c>
       <c r="X88" t="n">
-        <v>33446104.7414181</v>
+        <v>33256250.1323107</v>
       </c>
       <c r="Y88" t="n">
-        <v>6.68528398345308</v>
+        <v>6.63993277426351</v>
       </c>
     </row>
     <row r="89">
@@ -7670,22 +7670,22 @@
         <v>280429.34788386</v>
       </c>
       <c r="T89" t="n">
-        <v>671655.747849677</v>
+        <v>652505.442967918</v>
       </c>
       <c r="U89" t="n">
-        <v>8465214.66021454</v>
+        <v>8446064.35533278</v>
       </c>
       <c r="V89" t="n">
-        <v>1.67453734681984</v>
+        <v>2.0421984146383</v>
       </c>
       <c r="W89" t="n">
-        <v>6.19258662963021</v>
+        <v>6.83789052202663</v>
       </c>
       <c r="X89" t="n">
-        <v>33446104.7414181</v>
+        <v>33256250.1323107</v>
       </c>
       <c r="Y89" t="n">
-        <v>6.68528398345308</v>
+        <v>6.63993277426351</v>
       </c>
     </row>
     <row r="90">
@@ -7747,22 +7747,22 @@
         <v>264944.544888926</v>
       </c>
       <c r="T90" t="n">
-        <v>720104.412430397</v>
+        <v>653278.996377141</v>
       </c>
       <c r="U90" t="n">
-        <v>8759961.59517145</v>
+        <v>8693136.1791182</v>
       </c>
       <c r="V90" t="n">
-        <v>3.48186013926128</v>
+        <v>2.92528938202342</v>
       </c>
       <c r="W90" t="n">
-        <v>7.72343836940162</v>
+        <v>7.95843689698697</v>
       </c>
       <c r="X90" t="n">
-        <v>35800412.527964</v>
+        <v>35512673.6581571</v>
       </c>
       <c r="Y90" t="n">
-        <v>7.03910905245255</v>
+        <v>6.78496077239353</v>
       </c>
     </row>
     <row r="91">
@@ -7824,22 +7824,22 @@
         <v>307294.714619496</v>
       </c>
       <c r="T91" t="n">
-        <v>790965.281455801</v>
+        <v>746315.720705335</v>
       </c>
       <c r="U91" t="n">
-        <v>9062236.36238242</v>
+        <v>9017586.80163196</v>
       </c>
       <c r="V91" t="n">
-        <v>3.45064032446884</v>
+        <v>3.7322620493755</v>
       </c>
       <c r="W91" t="n">
-        <v>6.32440956535176</v>
+        <v>6.32873663122221</v>
       </c>
       <c r="X91" t="n">
-        <v>35800412.527964</v>
+        <v>35512673.6581571</v>
       </c>
       <c r="Y91" t="n">
-        <v>7.03910905245255</v>
+        <v>6.78496077239353</v>
       </c>
     </row>
     <row r="92">
@@ -7901,22 +7901,22 @@
         <v>288444.54442046</v>
       </c>
       <c r="T92" t="n">
-        <v>728169.864017042</v>
+        <v>651784.253853565</v>
       </c>
       <c r="U92" t="n">
-        <v>8873662.32079825</v>
+        <v>8797276.71063478</v>
       </c>
       <c r="V92" t="n">
-        <v>-2.08087754549137</v>
+        <v>-2.44311583402013</v>
       </c>
       <c r="W92" t="n">
-        <v>6.58034642398591</v>
+        <v>6.28541505823047</v>
       </c>
       <c r="X92" t="n">
-        <v>35800412.527964</v>
+        <v>35512673.6581571</v>
       </c>
       <c r="Y92" t="n">
-        <v>7.03910905245255</v>
+        <v>6.78496077239353</v>
       </c>
     </row>
     <row r="93">
@@ -7978,22 +7978,22 @@
         <v>320469.962409374</v>
       </c>
       <c r="T93" t="n">
-        <v>762931.318620251</v>
+        <v>663053.035780537</v>
       </c>
       <c r="U93" t="n">
-        <v>9104552.24961186</v>
+        <v>9004673.96677214</v>
       </c>
       <c r="V93" t="n">
-        <v>2.60196884292564</v>
+        <v>2.35751656972034</v>
       </c>
       <c r="W93" t="n">
-        <v>7.55252660516835</v>
+        <v>6.61384507550734</v>
       </c>
       <c r="X93" t="n">
-        <v>35800412.527964</v>
+        <v>35512673.6581571</v>
       </c>
       <c r="Y93" t="n">
-        <v>7.03910905245255</v>
+        <v>6.78496077239353</v>
       </c>
     </row>
     <row r="94">
@@ -8055,22 +8055,22 @@
         <v>281918.241991239</v>
       </c>
       <c r="T94" t="n">
-        <v>826146.838237586</v>
+        <v>625203.876360985</v>
       </c>
       <c r="U94" t="n">
-        <v>9132415.91129198</v>
+        <v>8931472.94941537</v>
       </c>
       <c r="V94" t="n">
-        <v>0.306040988246369</v>
+        <v>-0.812922462566475</v>
       </c>
       <c r="W94" t="n">
-        <v>4.25178023983371</v>
+        <v>2.74166613045458</v>
       </c>
       <c r="X94" t="n">
-        <v>36543338.7458852</v>
+        <v>35591550.3113616</v>
       </c>
       <c r="Y94" t="n">
-        <v>2.07518898655395</v>
+        <v>0.22210846179519</v>
       </c>
     </row>
     <row r="95">
@@ -8132,22 +8132,22 @@
         <v>302507.509914241</v>
       </c>
       <c r="T95" t="n">
-        <v>786672.682590286</v>
+        <v>537003.610737969</v>
       </c>
       <c r="U95" t="n">
-        <v>8925607.5134601</v>
+        <v>8675938.44160778</v>
       </c>
       <c r="V95" t="n">
-        <v>-2.26455299277558</v>
+        <v>-2.86105672888276</v>
       </c>
       <c r="W95" t="n">
-        <v>-1.50767253753691</v>
+        <v>-3.7886894525079</v>
       </c>
       <c r="X95" t="n">
-        <v>36543338.7458852</v>
+        <v>35591550.3113616</v>
       </c>
       <c r="Y95" t="n">
-        <v>2.07518898655395</v>
+        <v>0.22210846179519</v>
       </c>
     </row>
     <row r="96">
@@ -8209,22 +8209,22 @@
         <v>343857.765210638</v>
       </c>
       <c r="T96" t="n">
-        <v>878039.237582485</v>
+        <v>627521.829861496</v>
       </c>
       <c r="U96" t="n">
-        <v>9214977.16020796</v>
+        <v>8964459.75248697</v>
       </c>
       <c r="V96" t="n">
-        <v>3.24201625840574</v>
+        <v>3.32553432485768</v>
       </c>
       <c r="W96" t="n">
-        <v>3.84638075092994</v>
+        <v>1.90039539906812</v>
       </c>
       <c r="X96" t="n">
-        <v>36543338.7458852</v>
+        <v>35591550.3113616</v>
       </c>
       <c r="Y96" t="n">
-        <v>2.07518898655395</v>
+        <v>0.22210846179519</v>
       </c>
     </row>
     <row r="97">
@@ -8286,22 +8286,22 @@
         <v>342718.555035732</v>
       </c>
       <c r="T97" t="n">
-        <v>924773.701875647</v>
+        <v>674114.708801923</v>
       </c>
       <c r="U97" t="n">
-        <v>9270338.16092514</v>
+        <v>9019679.16785142</v>
       </c>
       <c r="V97" t="n">
-        <v>0.600771979731423</v>
+        <v>0.615981519121962</v>
       </c>
       <c r="W97" t="n">
-        <v>1.82091229494951</v>
+        <v>0.166637916427041</v>
       </c>
       <c r="X97" t="n">
-        <v>36543338.7458852</v>
+        <v>35591550.3113616</v>
       </c>
       <c r="Y97" t="n">
-        <v>2.07518898655395</v>
+        <v>0.22210846179519</v>
       </c>
     </row>
     <row r="98">
@@ -8363,22 +8363,22 @@
         <v>342475.452243925</v>
       </c>
       <c r="T98" t="n">
-        <v>864264.514080132</v>
+        <v>660843.845601949</v>
       </c>
       <c r="U98" t="n">
-        <v>9166902.08826694</v>
+        <v>8963481.41978876</v>
       </c>
       <c r="V98" t="n">
-        <v>-1.11577453662035</v>
+        <v>-0.623057062417086</v>
       </c>
       <c r="W98" t="n">
-        <v>0.377623810719376</v>
+        <v>0.358378405831459</v>
       </c>
       <c r="X98" t="n">
-        <v>36911150.2047262</v>
+        <v>36103680.798015</v>
       </c>
       <c r="Y98" t="n">
-        <v>1.00650753725242</v>
+        <v>1.43891030925375</v>
       </c>
     </row>
     <row r="99">
@@ -8440,22 +8440,22 @@
         <v>351829.159800379</v>
       </c>
       <c r="T99" t="n">
-        <v>868116.66496398</v>
+        <v>665731.54101938</v>
       </c>
       <c r="U99" t="n">
-        <v>9197006.7154138</v>
+        <v>8994621.5914692</v>
       </c>
       <c r="V99" t="n">
-        <v>0.328405680097691</v>
+        <v>0.347411571710256</v>
       </c>
       <c r="W99" t="n">
-        <v>3.04068044157692</v>
+        <v>3.67318362164823</v>
       </c>
       <c r="X99" t="n">
-        <v>36911150.2047262</v>
+        <v>36103680.798015</v>
       </c>
       <c r="Y99" t="n">
-        <v>1.00650753725242</v>
+        <v>1.43891030925375</v>
       </c>
     </row>
     <row r="100">
@@ -8517,22 +8517,22 @@
         <v>361299.078485411</v>
       </c>
       <c r="T100" t="n">
-        <v>871968.815847827</v>
+        <v>670619.23643681</v>
       </c>
       <c r="U100" t="n">
-        <v>9257001.79366557</v>
+        <v>9055652.21425455</v>
       </c>
       <c r="V100" t="n">
-        <v>0.652332656789483</v>
+        <v>0.678523517245372</v>
       </c>
       <c r="W100" t="n">
-        <v>0.456047071273026</v>
+        <v>1.01726667624649</v>
       </c>
       <c r="X100" t="n">
-        <v>36911150.2047262</v>
+        <v>36103680.798015</v>
       </c>
       <c r="Y100" t="n">
-        <v>1.00650753725242</v>
+        <v>1.43891030925375</v>
       </c>
     </row>
     <row r="101">
@@ -8594,22 +8594,22 @@
         <v>385926.304972178</v>
       </c>
       <c r="T101" t="n">
-        <v>875820.966731675</v>
+        <v>675506.93185424</v>
       </c>
       <c r="U101" t="n">
-        <v>9290239.60737989</v>
+        <v>9089925.57250246</v>
       </c>
       <c r="V101" t="n">
-        <v>0.359055928206341</v>
+        <v>0.378474762910573</v>
       </c>
       <c r="W101" t="n">
-        <v>0.214678753992339</v>
+        <v>0.778812675526371</v>
       </c>
       <c r="X101" t="n">
-        <v>36911150.2047262</v>
+        <v>36103680.798015</v>
       </c>
       <c r="Y101" t="n">
-        <v>1.00650753725242</v>
+        <v>1.43891030925375</v>
       </c>
     </row>
     <row r="102">
@@ -8671,22 +8671,22 @@
         <v>365508.923662228</v>
       </c>
       <c r="T102" t="n">
-        <v>879673.117615523</v>
+        <v>680394.62727167</v>
       </c>
       <c r="U102" t="n">
-        <v>9350636.99913358</v>
+        <v>9151358.50878972</v>
       </c>
       <c r="V102" t="n">
-        <v>0.650116620304463</v>
+        <v>0.675835415782779</v>
       </c>
       <c r="W102" t="n">
-        <v>2.00432936991665</v>
+        <v>2.09602809669676</v>
       </c>
       <c r="X102" t="n">
-        <v>37488966.6638237</v>
+        <v>36698065.9696498</v>
       </c>
       <c r="Y102" t="n">
-        <v>1.56542523300589</v>
+        <v>1.64632845875227</v>
       </c>
     </row>
     <row r="103">
@@ -8748,22 +8748,22 @@
         <v>382681.195671722</v>
       </c>
       <c r="T103" t="n">
-        <v>883525.268499371</v>
+        <v>685282.3226891</v>
       </c>
       <c r="U103" t="n">
-        <v>9359160.49123861</v>
+        <v>9160917.54542834</v>
       </c>
       <c r="V103" t="n">
-        <v>0.0911541331978227</v>
+        <v>0.104454837272896</v>
       </c>
       <c r="W103" t="n">
-        <v>1.76311468331372</v>
+        <v>1.84883768892354</v>
       </c>
       <c r="X103" t="n">
-        <v>37488966.6638237</v>
+        <v>36698065.9696498</v>
       </c>
       <c r="Y103" t="n">
-        <v>1.56542523300589</v>
+        <v>1.64632845875227</v>
       </c>
     </row>
     <row r="104">
@@ -8825,22 +8825,22 @@
         <v>393149.791932438</v>
       </c>
       <c r="T104" t="n">
-        <v>887377.419383219</v>
+        <v>690170.01810653</v>
       </c>
       <c r="U104" t="n">
-        <v>9416879.67243426</v>
+        <v>9219672.27115757</v>
       </c>
       <c r="V104" t="n">
-        <v>0.616713232449399</v>
+        <v>0.64136289228526</v>
       </c>
       <c r="W104" t="n">
-        <v>1.72710216906396</v>
+        <v>1.81124509888786</v>
       </c>
       <c r="X104" t="n">
-        <v>37488966.6638237</v>
+        <v>36698065.9696498</v>
       </c>
       <c r="Y104" t="n">
-        <v>1.56542523300589</v>
+        <v>1.64632845875227</v>
       </c>
     </row>
     <row r="105">
@@ -8902,22 +8902,22 @@
         <v>387842.087937949</v>
       </c>
       <c r="T105" t="n">
-        <v>891229.570267067</v>
+        <v>695057.713523961</v>
       </c>
       <c r="U105" t="n">
-        <v>9362289.50101724</v>
+        <v>9166117.64427414</v>
       </c>
       <c r="V105" t="n">
-        <v>-0.579705521530779</v>
+        <v>-0.580873433548897</v>
       </c>
       <c r="W105" t="n">
-        <v>0.775543976068381</v>
+        <v>0.838203472228273</v>
       </c>
       <c r="X105" t="n">
-        <v>37488966.6638237</v>
+        <v>36698065.9696498</v>
       </c>
       <c r="Y105" t="n">
-        <v>1.56542523300589</v>
+        <v>1.64632845875227</v>
       </c>
     </row>
     <row r="106">
@@ -8979,22 +8979,22 @@
         <v>402186.368143782</v>
       </c>
       <c r="T106" t="n">
-        <v>895081.721150914</v>
+        <v>699945.408941391</v>
       </c>
       <c r="U106" t="n">
-        <v>9511335.42770137</v>
+        <v>9316199.11549185</v>
       </c>
       <c r="V106" t="n">
-        <v>1.59198160522522</v>
+        <v>1.6373504796926</v>
       </c>
       <c r="W106" t="n">
-        <v>1.71858268674835</v>
+        <v>1.80126924919178</v>
       </c>
       <c r="X106" t="n">
-        <v>38216232.4729162</v>
+        <v>37441900.4912796</v>
       </c>
       <c r="Y106" t="n">
-        <v>1.93994626636204</v>
+        <v>2.02690387620167</v>
       </c>
     </row>
     <row r="107">
@@ -9056,22 +9056,22 @@
         <v>394419.448471462</v>
       </c>
       <c r="T107" t="n">
-        <v>898933.872034762</v>
+        <v>704833.104358821</v>
       </c>
       <c r="U107" t="n">
-        <v>9544507.10975323</v>
+        <v>9350406.34207729</v>
       </c>
       <c r="V107" t="n">
-        <v>0.34875945974155</v>
+        <v>0.367180071629808</v>
       </c>
       <c r="W107" t="n">
-        <v>1.9803765379184</v>
+        <v>2.06844779149344</v>
       </c>
       <c r="X107" t="n">
-        <v>38216232.4729162</v>
+        <v>37441900.4912796</v>
       </c>
       <c r="Y107" t="n">
-        <v>1.93994626636204</v>
+        <v>2.02690387620167</v>
       </c>
     </row>
     <row r="108">
@@ -9133,22 +9133,22 @@
         <v>404014.227193377</v>
       </c>
       <c r="T108" t="n">
-        <v>902786.02291861</v>
+        <v>709720.799776251</v>
       </c>
       <c r="U108" t="n">
-        <v>9556841.35423091</v>
+        <v>9363776.13108856</v>
       </c>
       <c r="V108" t="n">
-        <v>0.129228721146654</v>
+        <v>0.142986181799449</v>
       </c>
       <c r="W108" t="n">
-        <v>1.4862851248526</v>
+        <v>1.56300414692395</v>
       </c>
       <c r="X108" t="n">
-        <v>38216232.4729162</v>
+        <v>37441900.4912796</v>
       </c>
       <c r="Y108" t="n">
-        <v>1.93994626636204</v>
+        <v>2.02690387620167</v>
       </c>
     </row>
     <row r="109">
@@ -9210,22 +9210,22 @@
         <v>414175.176881635</v>
       </c>
       <c r="T109" t="n">
-        <v>906638.173802458</v>
+        <v>714608.495193681</v>
       </c>
       <c r="U109" t="n">
-        <v>9603548.58123073</v>
+        <v>9411518.90262195</v>
       </c>
       <c r="V109" t="n">
-        <v>0.488730797850232</v>
+        <v>0.509866648508224</v>
       </c>
       <c r="W109" t="n">
-        <v>2.57692394779364</v>
+        <v>2.67726498689562</v>
       </c>
       <c r="X109" t="n">
-        <v>38216232.4729162</v>
+        <v>37441900.4912796</v>
       </c>
       <c r="Y109" t="n">
-        <v>1.93994626636204</v>
+        <v>2.02690387620167</v>
       </c>
     </row>
     <row r="110">
@@ -9287,22 +9287,22 @@
         <v>401252.952974483</v>
       </c>
       <c r="T110" t="n">
-        <v>910490.324686306</v>
+        <v>719496.190611111</v>
       </c>
       <c r="U110" t="n">
-        <v>9663053.96918632</v>
+        <v>9472059.83511113</v>
       </c>
       <c r="V110" t="n">
-        <v>0.619618752925256</v>
+        <v>0.643264207569187</v>
       </c>
       <c r="W110" t="n">
-        <v>1.59513396029622</v>
+        <v>1.67300760414296</v>
       </c>
       <c r="X110" t="n">
-        <v>38768845.7135816</v>
+        <v>38011082.4444823</v>
       </c>
       <c r="Y110" t="n">
-        <v>1.44601705847633</v>
+        <v>1.52017377786478</v>
       </c>
     </row>
     <row r="111">
@@ -9364,22 +9364,22 @@
         <v>418925.931589126</v>
       </c>
       <c r="T111" t="n">
-        <v>914342.475570153</v>
+        <v>724383.886028541</v>
       </c>
       <c r="U111" t="n">
-        <v>9708522.22200272</v>
+        <v>9518563.63246111</v>
       </c>
       <c r="V111" t="n">
-        <v>0.470537088599415</v>
+        <v>0.490957596969576</v>
       </c>
       <c r="W111" t="n">
-        <v>1.71842411937532</v>
+        <v>1.79839553739077</v>
       </c>
       <c r="X111" t="n">
-        <v>38768845.7135816</v>
+        <v>38011082.4444823</v>
       </c>
       <c r="Y111" t="n">
-        <v>1.44601705847633</v>
+        <v>1.52017377786478</v>
       </c>
     </row>
     <row r="112">
@@ -9441,22 +9441,22 @@
         <v>414305.502041853</v>
       </c>
       <c r="T112" t="n">
-        <v>918194.626454001</v>
+        <v>729271.581445972</v>
       </c>
       <c r="U112" t="n">
-        <v>9704725.26486243</v>
+        <v>9515802.21985441</v>
       </c>
       <c r="V112" t="n">
-        <v>-0.0391095272118987</v>
+        <v>-0.0290108120650251</v>
       </c>
       <c r="W112" t="n">
-        <v>1.54741410001589</v>
+        <v>1.62355535456586</v>
       </c>
       <c r="X112" t="n">
-        <v>38768845.7135816</v>
+        <v>38011082.4444823</v>
       </c>
       <c r="Y112" t="n">
-        <v>1.44601705847633</v>
+        <v>1.52017377786478</v>
       </c>
     </row>
     <row r="113">
@@ -9518,22 +9518,22 @@
         <v>416165.094482685</v>
       </c>
       <c r="T113" t="n">
-        <v>922046.777337849</v>
+        <v>734159.276863402</v>
       </c>
       <c r="U113" t="n">
-        <v>9692544.25753011</v>
+        <v>9504656.75705566</v>
       </c>
       <c r="V113" t="n">
-        <v>-0.125516251103209</v>
+        <v>-0.117125834913698</v>
       </c>
       <c r="W113" t="n">
-        <v>0.926695747375277</v>
+        <v>0.989615548748101</v>
       </c>
       <c r="X113" t="n">
-        <v>38768845.7135816</v>
+        <v>38011082.4444823</v>
       </c>
       <c r="Y113" t="n">
-        <v>1.44601705847633</v>
+        <v>1.52017377786478</v>
       </c>
     </row>
     <row r="114">
@@ -9595,22 +9595,22 @@
         <v>427380.564246544</v>
       </c>
       <c r="T114" t="n">
-        <v>925898.928221697</v>
+        <v>739046.972280832</v>
       </c>
       <c r="U114" t="n">
-        <v>9808016.90031966</v>
+        <v>9621164.9443788</v>
       </c>
       <c r="V114" t="n">
-        <v>1.19135533170088</v>
+        <v>1.22580110256634</v>
       </c>
       <c r="W114" t="n">
-        <v>1.50017718617326</v>
+        <v>1.57415717239209</v>
       </c>
       <c r="X114" t="n">
-        <v>39448737.7105725</v>
+        <v>38707543.1540105</v>
       </c>
       <c r="Y114" t="n">
-        <v>1.753707092581</v>
+        <v>1.83225697543713</v>
       </c>
     </row>
     <row r="115">
@@ -9672,22 +9672,22 @@
         <v>416243.7556589</v>
       </c>
       <c r="T115" t="n">
-        <v>929751.079105545</v>
+        <v>743934.667698262</v>
       </c>
       <c r="U115" t="n">
-        <v>9872098.65862245</v>
+        <v>9686282.24721517</v>
       </c>
       <c r="V115" t="n">
-        <v>0.653361010223165</v>
+        <v>0.676813080461891</v>
       </c>
       <c r="W115" t="n">
-        <v>1.68487472016094</v>
+        <v>1.76201600609246</v>
       </c>
       <c r="X115" t="n">
-        <v>39448737.7105725</v>
+        <v>38707543.1540105</v>
       </c>
       <c r="Y115" t="n">
-        <v>1.753707092581</v>
+        <v>1.83225697543713</v>
       </c>
     </row>
     <row r="116">
@@ -9749,22 +9749,22 @@
         <v>430554.624882768</v>
       </c>
       <c r="T116" t="n">
-        <v>933603.229989393</v>
+        <v>748822.363115693</v>
       </c>
       <c r="U116" t="n">
-        <v>9859421.48240531</v>
+        <v>9674640.61553161</v>
       </c>
       <c r="V116" t="n">
-        <v>-0.12841419697592</v>
+        <v>-0.120186789796521</v>
       </c>
       <c r="W116" t="n">
-        <v>1.59402984959276</v>
+        <v>1.66920656826803</v>
       </c>
       <c r="X116" t="n">
-        <v>39448737.7105725</v>
+        <v>38707543.1540105</v>
       </c>
       <c r="Y116" t="n">
-        <v>1.753707092581</v>
+        <v>1.83225697543713</v>
       </c>
     </row>
     <row r="117">
@@ -9826,22 +9826,22 @@
         <v>429418.025186876</v>
       </c>
       <c r="T117" t="n">
-        <v>937455.380873241</v>
+        <v>753710.058533123</v>
       </c>
       <c r="U117" t="n">
-        <v>9909200.66922503</v>
+        <v>9725455.34688491</v>
       </c>
       <c r="V117" t="n">
-        <v>0.504889530370023</v>
+        <v>0.525236371795766</v>
       </c>
       <c r="W117" t="n">
-        <v>2.23528937230899</v>
+        <v>2.32305695484833</v>
       </c>
       <c r="X117" t="n">
-        <v>39448737.7105725</v>
+        <v>38707543.1540105</v>
       </c>
       <c r="Y117" t="n">
-        <v>1.753707092581</v>
+        <v>1.83225697543713</v>
       </c>
     </row>
   </sheetData>

</xml_diff>